<commit_message>
g maps locations load
</commit_message>
<xml_diff>
--- a/documentation/Obserwacje_model_danych.xlsx
+++ b/documentation/Obserwacje_model_danych.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DataEngineering\BIRD_PROJECTS\B1RDSPOT\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A52F133-CDB1-404E-8237-861FD3533597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB5E237-51C4-4EC0-BE8A-9851B9979D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="5400" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBSERVATION_FAC" sheetId="1" r:id="rId1"/>
     <sheet name="LOCATION_DETAILED_DIM" sheetId="2" r:id="rId2"/>
     <sheet name="LOCATION_DIM" sheetId="4" r:id="rId3"/>
     <sheet name="BIRD_SPECIE_DIM" sheetId="3" r:id="rId4"/>
+    <sheet name="STAGE.GOOGLE_MAPS_LOCATION" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>OBSERVATION_DATE</t>
   </si>
@@ -136,6 +137,12 @@
   </si>
   <si>
     <t>NOT  NULL</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>VARCHAR (64)</t>
   </si>
 </sst>
 </file>
@@ -667,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D1FB4E-84DE-4E41-8D2C-56D7FE83F95D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -739,4 +746,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E9AFCF-3134-4418-90E9-AD69877115AC}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
model update + bird data by year v2
</commit_message>
<xml_diff>
--- a/documentation/Obserwacje_model_danych.xlsx
+++ b/documentation/Obserwacje_model_danych.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DataEngineering\BIRD_PROJECTS\B1RDSPOT\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB5E237-51C4-4EC0-BE8A-9851B9979D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E613E4-2C0F-49FE-82B4-B88EEC0BFEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="5400" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6405" yWindow="5400" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OBSERVATION_FAC" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>OBSERVATION_DATE</t>
   </si>
@@ -115,9 +115,6 @@
     <t>BOOLEAN</t>
   </si>
   <si>
-    <t>IS_CERTAIN</t>
-  </si>
-  <si>
     <t>OBSERVATION_TYPE</t>
   </si>
   <si>
@@ -143,6 +140,15 @@
   </si>
   <si>
     <t>VARCHAR (64)</t>
+  </si>
+  <si>
+    <t>LOCATION_GENERAL</t>
+  </si>
+  <si>
+    <t>IS_UNSURE</t>
+  </si>
+  <si>
+    <t>DEFAULT 0</t>
   </si>
 </sst>
 </file>
@@ -462,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,16 +502,16 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -531,7 +537,7 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
         <v>27</v>
@@ -539,16 +545,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -609,10 +615,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -622,31 +628,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D89DE16-22B8-4F7A-8563-D50C558FF93F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -654,15 +664,18 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +750,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -752,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E9AFCF-3134-4418-90E9-AD69877115AC}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
@@ -764,7 +777,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -772,7 +785,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -780,10 +793,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>